<commit_message>
added cortex m3 to future work
</commit_message>
<xml_diff>
--- a/figures/nn_ops.xlsx
+++ b/figures/nn_ops.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10520"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/graham/Desktop/thesis/figures/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{073E73AB-08B7-9F49-AD3B-23F66DCC27F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{784656A8-3C2B-1743-8D89-97F75CF63822}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19960" yWindow="500" windowWidth="15960" windowHeight="20280" xr2:uid="{7B96BF8B-DAC3-1348-8829-EFAD386CBEE2}"/>
+    <workbookView xWindow="19880" yWindow="500" windowWidth="15960" windowHeight="20280" xr2:uid="{7B96BF8B-DAC3-1348-8829-EFAD386CBEE2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="22">
   <si>
     <t>Normalize</t>
   </si>
@@ -98,6 +98,9 @@
   </si>
   <si>
     <t>GOPS/W</t>
+  </si>
+  <si>
+    <t>STM32L152RE</t>
   </si>
 </sst>
 </file>
@@ -452,7 +455,7 @@
   <dimension ref="A1:J16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
+      <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -594,6 +597,23 @@
         <f t="shared" si="2"/>
         <v>6720</v>
       </c>
+      <c r="F5" t="s">
+        <v>21</v>
+      </c>
+      <c r="G5">
+        <v>1.0296E-2</v>
+      </c>
+      <c r="H5">
+        <v>1.0361910000000001</v>
+      </c>
+      <c r="I5">
+        <f>($D$16/H5)/1000000000</f>
+        <v>3.8210715978038794E-4</v>
+      </c>
+      <c r="J5">
+        <f>I5/G5</f>
+        <v>3.7112195005865184E-2</v>
+      </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" t="s">

</xml_diff>

<commit_message>
small edits to thesis + defense slides
</commit_message>
<xml_diff>
--- a/figures/nn_ops.xlsx
+++ b/figures/nn_ops.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/graham/Desktop/thesis/figures/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{784656A8-3C2B-1743-8D89-97F75CF63822}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FD47914-AA77-1F46-A545-616DDB329EDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="19880" yWindow="500" windowWidth="15960" windowHeight="20280" xr2:uid="{7B96BF8B-DAC3-1348-8829-EFAD386CBEE2}"/>
   </bookViews>
@@ -455,7 +455,7 @@
   <dimension ref="A1:J16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H24" sqref="H24"/>
+      <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -502,18 +502,18 @@
         <v>18</v>
       </c>
       <c r="G2">
-        <v>3.3984000000000002E-3</v>
+        <v>6.21917999999999E-3</v>
       </c>
       <c r="H2">
-        <v>3.1442009999999998</v>
+        <v>1.9610460000000001</v>
       </c>
       <c r="I2">
         <f t="shared" ref="I2:I3" si="0">($D$16/H2)/1000000000</f>
-        <v>1.2592579163991108E-4</v>
+        <v>2.0190041437069807E-4</v>
       </c>
       <c r="J2">
         <f t="shared" ref="J2:J3" si="1">I2/G2</f>
-        <v>3.7054434922290214E-2</v>
+        <v>3.2464153533214732E-2</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
@@ -535,18 +535,18 @@
         <v>17</v>
       </c>
       <c r="G3">
-        <v>3.9569440000000001E-4</v>
+        <v>4.1285099999999999E-4</v>
       </c>
       <c r="H3">
-        <v>0.26759803999999998</v>
+        <v>0.10091772</v>
       </c>
       <c r="I3">
         <f t="shared" si="0"/>
-        <v>1.4795923019466062E-3</v>
+        <v>3.9233545902543181E-3</v>
       </c>
       <c r="J3">
         <f t="shared" si="1"/>
-        <v>3.7392298246995819</v>
+        <v>9.5030763889498111</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
@@ -601,18 +601,18 @@
         <v>21</v>
       </c>
       <c r="G5">
-        <v>1.0296E-2</v>
+        <v>1.8693000000000001E-2</v>
       </c>
       <c r="H5">
-        <v>1.0361910000000001</v>
+        <v>0.16778596874999999</v>
       </c>
       <c r="I5">
         <f>($D$16/H5)/1000000000</f>
-        <v>3.8210715978038794E-4</v>
+        <v>2.3597682389636648E-3</v>
       </c>
       <c r="J5">
         <f>I5/G5</f>
-        <v>3.7112195005865184E-2</v>
+        <v>0.12623806981028537</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">

</xml_diff>